<commit_message>
using fixed closest mine
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -229,7 +229,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -272,7 +272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2384,11 +2384,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
+        <c:axId val="1585209472"/>
         <c:axId val="1585208688"/>
-        <c:axId val="1585211040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1585208688"/>
+        <c:axId val="1585209472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2430,7 +2430,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1585211040"/>
+        <c:crossAx val="1585208688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2438,7 +2438,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1585211040"/>
+        <c:axId val="1585208688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2489,7 +2489,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1585208688"/>
+        <c:crossAx val="1585209472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2900,11 +2900,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1585211824"/>
-        <c:axId val="1585209472"/>
+        <c:axId val="1585210648"/>
+        <c:axId val="1585211432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1585211824"/>
+        <c:axId val="1585210648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2946,7 +2946,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1585209472"/>
+        <c:crossAx val="1585211432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2954,7 +2954,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1585209472"/>
+        <c:axId val="1585211432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3005,7 +3005,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1585211824"/>
+        <c:crossAx val="1585210648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3386,11 +3386,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1585086776"/>
-        <c:axId val="1585087168"/>
+        <c:axId val="1585086384"/>
+        <c:axId val="1585092656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1585086776"/>
+        <c:axId val="1585086384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3432,7 +3432,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1585087168"/>
+        <c:crossAx val="1585092656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3440,7 +3440,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1585087168"/>
+        <c:axId val="1585092656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3491,7 +3491,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1585086776"/>
+        <c:crossAx val="1585086384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5618,11 +5618,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1585090696"/>
-        <c:axId val="1585084424"/>
+        <c:axId val="1585093440"/>
+        <c:axId val="1585088736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1585090696"/>
+        <c:axId val="1585093440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5664,7 +5664,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1585084424"/>
+        <c:crossAx val="1585088736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5672,7 +5672,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1585084424"/>
+        <c:axId val="1585088736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5723,7 +5723,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1585090696"/>
+        <c:crossAx val="1585093440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8047,7 +8047,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4F9D750E-EDF1-437F-82E2-A651B7C726A2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F9D750E-EDF1-437F-82E2-A651B7C726A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8088,7 +8088,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{29C5FA76-4716-46CF-A386-97C83E70700A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29C5FA76-4716-46CF-A386-97C83E70700A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8124,7 +8124,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E242ABE2-DF26-4730-B37A-F8EA8C4059CF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E242ABE2-DF26-4730-B37A-F8EA8C4059CF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8160,7 +8160,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C5840B41-17D0-4972-AA5C-E1F29FD09A19}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5840B41-17D0-4972-AA5C-E1F29FD09A19}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8478,11 +8478,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CE64"/>
+  <dimension ref="A1:CE66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BI7" sqref="BI7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AL66" sqref="AL66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15981,8 +15981,42 @@
         <v>5</v>
       </c>
     </row>
+    <row r="66" spans="2:50" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <f>AVERAGE(B64:J64)</f>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="N66">
+        <f>AVERAGE(N64:V64)</f>
+        <v>9</v>
+      </c>
+      <c r="Z66">
+        <f>AVERAGE(Z64:AH64)</f>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="AL66">
+        <f>AVERAGE(AL64:AT64)</f>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="AX66">
+        <f>AVERAGE(AX64:BF64)</f>
+        <v>15.333333333333334</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="AS62:AU62"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="I62:K62"/>
+    <mergeCell ref="M62:O62"/>
+    <mergeCell ref="Q62:S62"/>
+    <mergeCell ref="U62:W62"/>
+    <mergeCell ref="Y62:AA62"/>
+    <mergeCell ref="AC62:AE62"/>
+    <mergeCell ref="AG62:AI62"/>
+    <mergeCell ref="AK62:AM62"/>
+    <mergeCell ref="AO62:AQ62"/>
     <mergeCell ref="BU62:BW62"/>
     <mergeCell ref="BY62:CA62"/>
     <mergeCell ref="CC62:CE62"/>
@@ -15992,18 +16026,6 @@
     <mergeCell ref="BI62:BK62"/>
     <mergeCell ref="BM62:BO62"/>
     <mergeCell ref="BQ62:BS62"/>
-    <mergeCell ref="Y62:AA62"/>
-    <mergeCell ref="AC62:AE62"/>
-    <mergeCell ref="AG62:AI62"/>
-    <mergeCell ref="AK62:AM62"/>
-    <mergeCell ref="AO62:AQ62"/>
-    <mergeCell ref="AS62:AU62"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="I62:K62"/>
-    <mergeCell ref="M62:O62"/>
-    <mergeCell ref="Q62:S62"/>
-    <mergeCell ref="U62:W62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>